<commit_message>
included las participant, excluded 20 min participant
</commit_message>
<xml_diff>
--- a/RESULTS/Round1/_free_text_answers.xlsx
+++ b/RESULTS/Round1/_free_text_answers.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1215">
   <si>
     <t xml:space="preserve">index</t>
   </si>
@@ -2558,586 +2558,589 @@
     <t xml:space="preserve">I have no idea about the goal of this experiement as I found it impossible to sort the cards correctly. I could not find a correlation between colour, shapes, or number of shapes.</t>
   </si>
   <si>
+    <t xml:space="preserve">I have absolutely no idea!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I could not find a rule.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Being able to find a patten within the card sorting game. Since mataching the cards by colour or shape didn't work. I was very confused for quite sometime.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have nothing more to add. (-:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do it in order once you have established a patten within the cards. As if you were sorting the cards through numbers. 1&gt;2&gt;3&gt;4. Then go back to sorting the first card at number one again and repeat the patten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how long it took to get the sequence correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventually, more through luck than anything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A very interesting study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfortunately not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how long it takes to find pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequential order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To drive me potty!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No :(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern finding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It would have been great if you showed the solution at the end!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From what I remember, it was a sequential pattern by colour I think</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To determine if people could find a pattern, and if not if they became frustrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thank you for a fun study!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every time I thought I did it changed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If I remember correctly, I think the goal was to see if we could adapt to changing situations or rules with the same set of materials. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I honestly did not. Nearly any kind of pattern I tried to interpret, didn't provide any kind of consistency. Color, shape, it felt like there were multiple rules just for a single combination, and it was honestly too much to keep in my head. I'd really like to know, because of all my time on Prolific and other platforms, I've never done a card sort game this difficult.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how different people spot patterns in repeating scenarios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">interesting (:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no. Maybe colours or numbers of shapes?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see if I could find a connection to sorting the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, simply to sort in order from left to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frustration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm glad I found the rule in the end, I was trying to find a hard solution when in reality it was so simple!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes we just had to add the cards in a row left to right!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i had no idea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To find a pattern, to see how fast people can find a pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was an interesting twist!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. It wasn't about matching but about going across from left to right in order one card after another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how quickly people can pick up a pattern and solve a problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes - to deal from left to right continuously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To work out how to sort the cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No I didn't, annoyingly. I'd like to know the answer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how long it would take to figure out how to sort the cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wish I'd figured it out sooner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, just taking turns to each pile from left to right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goal of experiment was to find the solution of a problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how quickly you pick up the pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It went 1,2,3,4 as in the first section ,next card goes in the next section etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moonsq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To figure out you had to put the cards on the piles in a 1, 2, 3, 4 pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fun little game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 2, 3, 4, that was the rule. I thought at first it was to do with moons and stars or 4 then 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I honestly cant think of a goal I achieved while doing that.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rule was to start on the left and move right covering each key card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frustration of the participant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I thought my computer was not working correctly - still not convinced that it was alright.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibly - order of 2nd card, third card, fourth card, first card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeing if random patterns affecting the choice of card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not throughout, but then at the end they went from left to right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To work out the rule to the card game without being given any instruction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, To start from 1 to 4 and place them accordingly on each card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To assess how you picked the cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I thought there was but it changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See how long I would do the experiment as I kept getting incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No rule until the end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really honestly don't know, may be the level of perserveance of the participant!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I feel I must be not an overly confident person as I would just like to know for sure that I managed to find the correct way.  I think it took me a little while also as with other studies they often give you examples and I was assuming that this would be the case however you were straight in wondering what was going wrong!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think so, though it would be nice to have it clarified.  Eventually it seemed that if I dealt the cards from left to right it seemed to work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how long it takes people to work out correct sequence of card dealing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. Deal from the deck to the first key card, then the 2nd, then the 3rd and then the fourth and repeat till call the deck of cards are used up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It one's patience, understanding and moving of cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No I did not. It seemed very randomly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsure, found it quite confusing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the pack left to right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think the goal  was to see if it's possible to figure out the rules of the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The card from a deck had to be sorted firstly to the card on the left and have the colors match some of the pattern from the deck card. Then the same had to be done for the card next to the left one and so on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've absolutely no idea!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I did not sorry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the goal was to sort the moons card in the different cards and see if the individual formed an pattern depending on correct or incorrect selections, if the individual formed an sequence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an rule to try each card and see if it matched, process of elimination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether people find a correlation in an experiment when there might not be a correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By the end, sorting the cards from 1-4 in order seemed to work but it doesn't seem apparent as an actual rule, instead rather random.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was to see how people detect patterns and follow them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rule was to start with the third card from the left and continue left to right, starting over at the end of the row.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to see if people would give up trying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more than one round would be interesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 2, 3, 4 - according to the number of shapes on the card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am unsure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, the card should be dragged to the first card to the left, then second one, third one then fourth one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See how long it would take us to figure out the rule to sorting the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No further comments.  Everything worked great.  Good luck with your research!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The correct sort is a repeating pattern from left to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To drag and drop cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to discover any set rule to correctly place card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sometimes going down the line or up the line appeared to work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see if you can understand how the cards should be sorted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">just go 1,2,3,4 and then repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To work out the sequence of the cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only part I think,  Certain cards should be placed by their house value being counted on from the value of the previous Correct card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To try and find a pattern in the cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put them on the next card left to right and repeat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to rememeber patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes it was the image we originally saw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to test my level of frustration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">put the cards onto the piles starting at the left hand pile and continuing across then back to the first pile again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see if I thought there was a 'winning' pattern that was correct, and how I reacted to any patterns of correct answers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Towards the end it was correct to follow a pattern of selecting each of the colours in a set order, but I didn't find any rule for the majority of the test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">something about positive feedback and methods?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nope! Very frustrating!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To try and ascertain an order for the cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue, green, red and then yellow although i think sometimes, the yellow wasn't included. The majority started blue then green.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How quick people are in deciphering a pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great survey. Did enjoy it. Kudos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes i did. There was a pattern for placing the cards with involved a clockwise placement of the card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To measure how quickly I determined the rule for sorting the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At first, I thought it was random. But towards the end, I noticed that the order was simply left-to-right repeated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how many people will see a rule for sorting the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It just moved always 1 card to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have no idea, I found it hard to figure out what I was doing to be honest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did as best I could but was very unsure how to work out the sorting rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it seemed to work in the order of 1, 2, 3, 4, 5 but I really didn't know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To figure out the rule of how to sort the cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, move to the right once each time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuition?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I misunderstood, I was moving the coloured cards over the card at the bottom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In sequence 4-3-2-1 then start at 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventually left to right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how long it would take to work out the pattern and what patterns people apply first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, the rule was 1,2,3,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To test memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think so, it was basically in order from left to right towards the end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i'm sorry about that i couldn't find the main goal of this experiment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thanks for the study it was fun for me.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes. it was all bout the algorithm of correct order of shape.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How long it takes individuals to spot a pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, the cards were sorted from left to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't know.  it didn't really work because nothing on the moon card changed and shapes and colours were irrelevant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annoying because no feedback on the page; i thought the game wasn't working and almost closed it a few times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">went from left to right.  tested wrong places and then went to where it should have been assuming i had carried on in order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do detect patterns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes - place one card on the first card above, second on the second card, then on the third card and so on. once a card has been placed on all four cards, start back on the first pile of cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRYING TO ANNOY AND FRUSTRATE THE PLAYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To uncover the order through trial and error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tricky until the pattern was realised, then very easy from then onwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 1-4 repeating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfect thanks. sorting cards into deck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no, i loved it. thanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For people to try and be able to remember the correct order of the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes I started from right to left, one by one I was able to then remember the correct order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how long it took for participants to work out the rule so they could be compared by gender, age and their vision characteristics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes.The correct one was ascending left to right &amp;amp; then would start again at the leftmost pack in a loop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see if i was paying attention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drag the card on the key cards in order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I literally have no idea. To test patience?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After trying every conceivable combination I realised it went left to right - left to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left to right in ascending number of shapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to see if you could work out the pattern of the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the pattern move across from left to right and then back to start at the left again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The goal of the experiment was to sort out some card from a deck of cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I did not see any correlation of this experiment with colour blindness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I found out a rule of sorting the cards. Once you sort out the first card from the deck of cards correctly, you are sure to sort out the next card correctly as well. I found that in the middle of the experiement although I still made a bit of a mess in between sorting the cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figuring out a pattern?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was determined by the number of objects on the key cards, following the order of 3, 4, 1 and finally 2. So nothing to do with the actual shapes or colour of the key cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If one can spot a pattern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribute a card from the deck to each of the top cards from left to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The goal of the experiment was to observe how people develop different strategies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The experiment was confusing in the beginning, but I got the hang of it. Thank you!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorting the cards in sequential order proved to work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can only vaguely remember it but I don't think I could see any obvious pattern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial and error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how the test subject changes strategy over the course of the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drag it to the cards in order of left to right then repeating this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patience on how long people would take to become frustrated and quit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am not too sure if I completed it correctly or was just shuffling the cards up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think the cards were just in order starting from the second card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to indicate the correct order of the cards matching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incredibly irritating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No I didn't, not even sure I was doing it correctly . Might have been something with adding up to 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to find the correct sorting pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes. place the first card on the 2nd card along, the next on the 3rd, the next on the 4th, next on 1st and repeat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see how long it would take me to work out the pattern?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wear glasses that correct my vision. At first I thought it might be to do with the colours and then I felt that Ah aha! moment. That is such a good way to describe it as that is exactly how I felt :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, the cards went clockwise. So if I put the card on 1 then the next time I would put it on the 2nd card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No idea!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was confused I only saw the same card. I thought I need to sort different cards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, I had to put the card to the first, after the second, after the third and finally the fourth card, in turns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To figure out patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seemed to go in sequential order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it went in order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How long it took someone to realise the sequence of cards,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventually I (think ) I worked out that each card was just in sequence moving it to the pile one by one. This I think was my A-ha moment. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Not sure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No i did not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have absolutely no idea!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I could not find a rule.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Being able to find a patten within the card sorting game. Since mataching the cards by colour or shape didn't work. I was very confused for quite sometime.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have nothing more to add. (-:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do it in order once you have established a patten within the cards. As if you were sorting the cards through numbers. 1&gt;2&gt;3&gt;4. Then go back to sorting the first card at number one again and repeat the patten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how long it took to get the sequence correct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eventually, more through luck than anything</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A very interesting study.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unfortunately not.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">how long it takes to find pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequential order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To drive me potty!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No :(</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pattern finding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It would have been great if you showed the solution at the end!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From what I remember, it was a sequential pattern by colour I think</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To determine if people could find a pattern, and if not if they became frustrated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thank you for a fun study!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Every time I thought I did it changed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If I remember correctly, I think the goal was to see if we could adapt to changing situations or rules with the same set of materials. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank you.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I honestly did not. Nearly any kind of pattern I tried to interpret, didn't provide any kind of consistency. Color, shape, it felt like there were multiple rules just for a single combination, and it was honestly too much to keep in my head. I'd really like to know, because of all my time on Prolific and other platforms, I've never done a card sort game this difficult.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how different people spot patterns in repeating scenarios </t>
-  </si>
-  <si>
-    <t xml:space="preserve">interesting (:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no. Maybe colours or numbers of shapes?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see if I could find a connection to sorting the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, simply to sort in order from left to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frustration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I'm glad I found the rule in the end, I was trying to find a hard solution when in reality it was so simple!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes we just had to add the cards in a row left to right!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i had no idea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To find a pattern, to see how fast people can find a pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It was an interesting twist!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes. It wasn't about matching but about going across from left to right in order one card after another.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how quickly people can pick up a pattern and solve a problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes - to deal from left to right continuously</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To work out how to sort the cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No I didn't, annoyingly. I'd like to know the answer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how long it would take to figure out how to sort the cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I wish I'd figured it out sooner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, just taking turns to each pile from left to right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goal of experiment was to find the solution of a problem.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moonsq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To figure out you had to put the cards on the piles in a 1, 2, 3, 4 pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fun little game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, 2, 3, 4, that was the rule. I thought at first it was to do with moons and stars or 4 then 5.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I honestly cant think of a goal I achieved while doing that.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The rule was to start on the left and move right covering each key card.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frustration of the participant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I thought my computer was not working correctly - still not convinced that it was alright.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibly - order of 2nd card, third card, fourth card, first card.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seeing if random patterns affecting the choice of card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not throughout, but then at the end they went from left to right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To work out the rule to the card game without being given any instruction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, To start from 1 to 4 and place them accordingly on each card.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To assess how you picked the cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I thought there was but it changed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See how long I would do the experiment as I kept getting incorrect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No rule until the end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I really honestly don't know, may be the level of perserveance of the participant!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I feel I must be not an overly confident person as I would just like to know for sure that I managed to find the correct way.  I think it took me a little while also as with other studies they often give you examples and I was assuming that this would be the case however you were straight in wondering what was going wrong!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think so, though it would be nice to have it clarified.  Eventually it seemed that if I dealt the cards from left to right it seemed to work.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how long it takes people to work out correct sequence of card dealing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes. Deal from the deck to the first key card, then the 2nd, then the 3rd and then the fourth and repeat till call the deck of cards are used up.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It one's patience, understanding and moving of cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No I did not. It seemed very randomly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unsure, found it quite confusing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow the pack left to right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think the goal  was to see if it's possible to figure out the rules of the game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The card from a deck had to be sorted firstly to the card on the left and have the colors match some of the pattern from the deck card. Then the same had to be done for the card next to the left one and so on.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I've absolutely no idea!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I did not sorry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the goal was to sort the moons card in the different cards and see if the individual formed an pattern depending on correct or incorrect selections, if the individual formed an sequence.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">an rule to try each card and see if it matched, process of elimination.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether people find a correlation in an experiment when there might not be a correlation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By the end, sorting the cards from 1-4 in order seemed to work but it doesn't seem apparent as an actual rule, instead rather random.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It was to see how people detect patterns and follow them.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The rule was to start with the third card from the left and continue left to right, starting over at the end of the row.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to see if people would give up trying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">more than one round would be interesting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, 2, 3, 4 - according to the number of shapes on the card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I am unsure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, the card should be dragged to the first card to the left, then second one, third one then fourth one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See how long it would take us to figure out the rule to sorting the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No further comments.  Everything worked great.  Good luck with your research!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The correct sort is a repeating pattern from left to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To drag and drop cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to discover any set rule to correctly place card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sometimes going down the line or up the line appeared to work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see if you can understand how the cards should be sorted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank you!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">just go 1,2,3,4 and then repeat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To work out the sequence of the cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only part I think,  Certain cards should be placed by their house value being counted on from the value of the previous Correct card.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To try and find a pattern in the cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Put them on the next card left to right and repeat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to rememeber patterns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes it was the image we originally saw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to test my level of frustration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">put the cards onto the piles starting at the left hand pile and continuing across then back to the first pile again</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see if I thought there was a 'winning' pattern that was correct, and how I reacted to any patterns of correct answers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Towards the end it was correct to follow a pattern of selecting each of the colours in a set order, but I didn't find any rule for the majority of the test.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">something about positive feedback and methods?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nope! Very frustrating!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To try and ascertain an order for the cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue, green, red and then yellow although i think sometimes, the yellow wasn't included. The majority started blue then green.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How quick people are in deciphering a pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great survey. Did enjoy it. Kudos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes i did. There was a pattern for placing the cards with involved a clockwise placement of the card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To measure how quickly I determined the rule for sorting the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At first, I thought it was random. But towards the end, I noticed that the order was simply left-to-right repeated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how many people will see a rule for sorting the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It just moved always 1 card to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have no idea, I found it hard to figure out what I was doing to be honest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did as best I could but was very unsure how to work out the sorting rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it seemed to work in the order of 1, 2, 3, 4, 5 but I really didn't know</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To figure out the rule of how to sort the cars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, move to the right once each time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intuition?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I misunderstood, I was moving the coloured cards over the card at the bottom.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In sequence 4-3-2-1 then start at 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eventually left to right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">how long it would take to work out the pattern and what patterns people apply first</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, the rule was 1,2,3,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNSURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To test memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think so, it was basically in order from left to right towards the end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i'm sorry about that i couldn't find the main goal of this experiment.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thanks for the study it was fun for me.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes. it was all bout the algorithm of correct order of shape.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How long it takes individuals to spot a pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, the cards were sorted from left to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">don't know.  it didn't really work because nothing on the moon card changed and shapes and colours were irrelevant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annoying because no feedback on the page; i thought the game wasn't working and almost closed it a few times</t>
-  </si>
-  <si>
-    <t xml:space="preserve">went from left to right.  tested wrong places and then went to where it should have been assuming i had carried on in order.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do detect patterns.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes - place one card on the first card above, second on the second card, then on the third card and so on. once a card has been placed on all four cards, start back on the first pile of cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRYING TO ANNOY AND FRUSTRATE THE PLAYER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To uncover the order through trial and error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tricky until the pattern was realised, then very easy from then onwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 1-4 repeating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perfect thanks. sorting cards into deck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no, i loved it. thanks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For people to try and be able to remember the correct order of the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Worked well</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes I started from right to left, one by one I was able to then remember the correct order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how long it took for participants to work out the rule so they could be compared by gender, age and their vision characteristics.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes.The correct one was ascending left to right &amp;amp; then would start again at the leftmost pack in a loop.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see if i was paying attention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drag the card on the key cards in order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I literally have no idea. To test patience?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After trying every conceivable combination I realised it went left to right - left to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">left to right in ascending number of shapes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to see if you could work out the pattern of the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the pattern move across from left to right and then back to start at the left again</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The goal of the experiment was to sort out some card from a deck of cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I did not see any correlation of this experiment with colour blindness.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I found out a rule of sorting the cards. Once you sort out the first card from the deck of cards correctly, you are sure to sort out the next card correctly as well. I found that in the middle of the experiement although I still made a bit of a mess in between sorting the cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Figuring out a pattern?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It was determined by the number of objects on the key cards, following the order of 3, 4, 1 and finally 2. So nothing to do with the actual shapes or colour of the key cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If one can spot a pattern.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distribute a card from the deck to each of the top cards from left to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The goal of the experiment was to observe how people develop different strategies.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The experiment was confusing in the beginning, but I got the hang of it. Thank you!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorting the cards in sequential order proved to work.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I can only vaguely remember it but I don't think I could see any obvious pattern.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trial and error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how the test subject changes strategy over the course of the game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drag it to the cards in order of left to right then repeating this.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patience on how long people would take to become frustrated and quit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I am not too sure if I completed it correctly or was just shuffling the cards up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think the cards were just in order starting from the second card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to indicate the correct order of the cards matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incredibly irritating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No I didn't, not even sure I was doing it correctly . Might have been something with adding up to 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to find the correct sorting pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes. place the first card on the 2nd card along, the next on the 3rd, the next on the 4th, next on 1st and repeat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To see how long it would take me to work out the pattern?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I wear glasses that correct my vision. At first I thought it might be to do with the colours and then I felt that Ah aha! moment. That is such a good way to describe it as that is exactly how I felt :)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, the cards went clockwise. So if I put the card on 1 then the next time I would put it on the 2nd card.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No idea!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I was confused I only saw the same card. I thought I need to sort different cards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, I had to put the card to the first, after the second, after the third and finally the fourth card, in turns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To figure out patterns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It seemed to go in sequential order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it went in order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How long it took someone to realise the sequence of cards,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eventually I (think ) I worked out that each card was just in sequence moving it to the pile one by one. This I think was my A-ha moment. </t>
   </si>
   <si>
     <t xml:space="preserve">I think the goal of the experiment was to test our strategy.</t>
@@ -13683,7 +13686,7 @@
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>769</v>
+        <v>783</v>
       </c>
       <c r="B374" t="s">
         <v>730</v>
@@ -13692,16 +13695,16 @@
         <v>0</v>
       </c>
       <c r="D374" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E374" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F374" t="s">
         <v>848</v>
       </c>
       <c r="G374" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="H374" t="s">
         <v>849</v>
@@ -13709,33 +13712,33 @@
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>783</v>
+        <v>790</v>
       </c>
       <c r="B375" t="s">
         <v>730</v>
       </c>
       <c r="C375" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D375" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E375" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F375" t="s">
         <v>850</v>
       </c>
       <c r="G375" t="s">
-        <v>10</v>
+        <v>851</v>
       </c>
       <c r="H375" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>790</v>
+        <v>797</v>
       </c>
       <c r="B376" t="s">
         <v>730</v>
@@ -13747,13 +13750,13 @@
         <v>1</v>
       </c>
       <c r="E376" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F376" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="G376" t="s">
-        <v>853</v>
+        <v>10</v>
       </c>
       <c r="H376" t="s">
         <v>854</v>
@@ -13761,25 +13764,25 @@
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="B377" t="s">
         <v>730</v>
       </c>
       <c r="C377" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D377" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E377" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F377" t="s">
+        <v>428</v>
+      </c>
+      <c r="G377" t="s">
         <v>855</v>
-      </c>
-      <c r="G377" t="s">
-        <v>10</v>
       </c>
       <c r="H377" t="s">
         <v>856</v>
@@ -13787,25 +13790,25 @@
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>804</v>
+        <v>818</v>
       </c>
       <c r="B378" t="s">
         <v>730</v>
       </c>
       <c r="C378" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D378" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E378" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F378" t="s">
-        <v>428</v>
+        <v>857</v>
       </c>
       <c r="G378" t="s">
-        <v>857</v>
+        <v>10</v>
       </c>
       <c r="H378" t="s">
         <v>858</v>
@@ -13813,19 +13816,19 @@
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>818</v>
+        <v>841</v>
       </c>
       <c r="B379" t="s">
         <v>730</v>
       </c>
       <c r="C379" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D379" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E379" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F379" t="s">
         <v>859</v>
@@ -13839,59 +13842,59 @@
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B380" t="s">
         <v>730</v>
       </c>
       <c r="C380" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D380" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E380" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F380" t="s">
         <v>861</v>
       </c>
       <c r="G380" t="s">
-        <v>10</v>
+        <v>862</v>
       </c>
       <c r="H380" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B381" t="s">
         <v>730</v>
       </c>
       <c r="C381" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D381" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E381" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F381" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="G381" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H381" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>843</v>
+        <v>849</v>
       </c>
       <c r="B382" t="s">
         <v>730</v>
@@ -13906,18 +13909,18 @@
         <v>10</v>
       </c>
       <c r="F382" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="G382" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="H382" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="B383" t="s">
         <v>730</v>
@@ -13929,39 +13932,39 @@
         <v>0</v>
       </c>
       <c r="E383" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F383" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="G383" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="H383" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>853</v>
+        <v>869</v>
       </c>
       <c r="B384" t="s">
         <v>730</v>
       </c>
       <c r="C384" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D384" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E384" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F384" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G384" t="s">
-        <v>873</v>
+        <v>10</v>
       </c>
       <c r="H384" t="s">
         <v>874</v>
@@ -13969,7 +13972,7 @@
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>869</v>
+        <v>884</v>
       </c>
       <c r="B385" t="s">
         <v>730</v>
@@ -13981,73 +13984,73 @@
         <v>1</v>
       </c>
       <c r="E385" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F385" t="s">
         <v>875</v>
       </c>
       <c r="G385" t="s">
-        <v>10</v>
+        <v>876</v>
       </c>
       <c r="H385" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>884</v>
+        <v>889</v>
       </c>
       <c r="B386" t="s">
         <v>730</v>
       </c>
       <c r="C386" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D386" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E386" t="n">
         <v>7</v>
       </c>
       <c r="F386" t="s">
-        <v>877</v>
+        <v>818</v>
       </c>
       <c r="G386" t="s">
+        <v>10</v>
+      </c>
+      <c r="H386" t="s">
         <v>878</v>
-      </c>
-      <c r="H386" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>889</v>
+        <v>898</v>
       </c>
       <c r="B387" t="s">
         <v>730</v>
       </c>
       <c r="C387" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D387" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E387" t="n">
         <v>7</v>
       </c>
       <c r="F387" t="s">
-        <v>818</v>
+        <v>879</v>
       </c>
       <c r="G387" t="s">
-        <v>10</v>
+        <v>880</v>
       </c>
       <c r="H387" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>898</v>
+        <v>912</v>
       </c>
       <c r="B388" t="s">
         <v>730</v>
@@ -14062,10 +14065,10 @@
         <v>7</v>
       </c>
       <c r="F388" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="G388" t="s">
-        <v>882</v>
+        <v>67</v>
       </c>
       <c r="H388" t="s">
         <v>883</v>
@@ -14073,25 +14076,25 @@
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="B389" t="s">
         <v>730</v>
       </c>
       <c r="C389" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D389" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E389" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F389" t="s">
         <v>884</v>
       </c>
       <c r="G389" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="H389" t="s">
         <v>885</v>
@@ -14099,80 +14102,80 @@
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B390" t="s">
         <v>730</v>
       </c>
       <c r="C390" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D390" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E390" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F390" t="s">
         <v>886</v>
       </c>
       <c r="G390" t="s">
-        <v>10</v>
+        <v>887</v>
       </c>
       <c r="H390" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>916</v>
+        <v>933</v>
       </c>
       <c r="B391" t="s">
         <v>730</v>
       </c>
       <c r="C391" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D391" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E391" t="n">
         <v>7</v>
       </c>
       <c r="F391" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="G391" t="s">
-        <v>889</v>
+        <v>121</v>
       </c>
       <c r="H391" t="s">
-        <v>890</v>
+        <v>394</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B392" t="s">
         <v>730</v>
       </c>
       <c r="C392" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D392" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E392" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F392" t="s">
+        <v>890</v>
+      </c>
+      <c r="G392" t="s">
+        <v>10</v>
+      </c>
+      <c r="H392" t="s">
         <v>891</v>
-      </c>
-      <c r="G392" t="s">
-        <v>121</v>
-      </c>
-      <c r="H392" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="393">
@@ -16012,13 +16015,13 @@
         <v>7</v>
       </c>
       <c r="F463" t="s">
-        <v>848</v>
+        <v>1042</v>
       </c>
       <c r="G463" t="s">
         <v>121</v>
       </c>
       <c r="H463" t="s">
-        <v>848</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="464">
@@ -16038,13 +16041,13 @@
         <v>7</v>
       </c>
       <c r="F464" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="G464" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="H464" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="465">
@@ -16064,13 +16067,13 @@
         <v>4</v>
       </c>
       <c r="F465" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="G465" t="s">
         <v>10</v>
       </c>
       <c r="H465" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="466">
@@ -16090,13 +16093,13 @@
         <v>6</v>
       </c>
       <c r="F466" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="G466" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="H466" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="467">
@@ -16116,13 +16119,13 @@
         <v>8</v>
       </c>
       <c r="F467" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="G467" t="s">
         <v>10</v>
       </c>
       <c r="H467" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="468">
@@ -16168,13 +16171,13 @@
         <v>3</v>
       </c>
       <c r="F469" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="G469" t="s">
         <v>121</v>
       </c>
       <c r="H469" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="470">
@@ -16194,13 +16197,13 @@
         <v>7</v>
       </c>
       <c r="F470" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="G470" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="H470" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="471">
@@ -16220,13 +16223,13 @@
         <v>2</v>
       </c>
       <c r="F471" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="G471" t="s">
         <v>121</v>
       </c>
       <c r="H471" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="472">
@@ -16234,7 +16237,7 @@
         <v>7</v>
       </c>
       <c r="B472" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C472" t="b">
         <v>1</v>
@@ -16246,13 +16249,13 @@
         <v>2</v>
       </c>
       <c r="F472" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="G472" t="s">
         <v>10</v>
       </c>
       <c r="H472" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="473">
@@ -16260,7 +16263,7 @@
         <v>14</v>
       </c>
       <c r="B473" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C473" t="b">
         <v>1</v>
@@ -16272,13 +16275,13 @@
         <v>1</v>
       </c>
       <c r="F473" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="G473" t="s">
         <v>10</v>
       </c>
       <c r="H473" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="474">
@@ -16286,7 +16289,7 @@
         <v>21</v>
       </c>
       <c r="B474" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C474" t="b">
         <v>1</v>
@@ -16298,7 +16301,7 @@
         <v>2</v>
       </c>
       <c r="F474" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="G474" t="s">
         <v>10</v>
@@ -16312,7 +16315,7 @@
         <v>35</v>
       </c>
       <c r="B475" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C475" t="b">
         <v>1</v>
@@ -16330,7 +16333,7 @@
         <v>143</v>
       </c>
       <c r="H475" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="476">
@@ -16338,7 +16341,7 @@
         <v>42</v>
       </c>
       <c r="B476" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C476" t="b">
         <v>1</v>
@@ -16350,13 +16353,13 @@
         <v>1</v>
       </c>
       <c r="F476" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="G476" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="H476" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="477">
@@ -16364,7 +16367,7 @@
         <v>49</v>
       </c>
       <c r="B477" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C477" t="b">
         <v>1</v>
@@ -16390,7 +16393,7 @@
         <v>63</v>
       </c>
       <c r="B478" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C478" t="b">
         <v>1</v>
@@ -16402,13 +16405,13 @@
         <v>1</v>
       </c>
       <c r="F478" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="G478" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="H478" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="479">
@@ -16416,7 +16419,7 @@
         <v>70</v>
       </c>
       <c r="B479" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C479" t="b">
         <v>1</v>
@@ -16428,13 +16431,13 @@
         <v>1</v>
       </c>
       <c r="F479" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="G479" t="s">
         <v>10</v>
       </c>
       <c r="H479" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="480">
@@ -16442,7 +16445,7 @@
         <v>77</v>
       </c>
       <c r="B480" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C480" t="b">
         <v>1</v>
@@ -16457,10 +16460,10 @@
         <v>123</v>
       </c>
       <c r="G480" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="H480" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="481">
@@ -16468,7 +16471,7 @@
         <v>84</v>
       </c>
       <c r="B481" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C481" t="b">
         <v>1</v>
@@ -16480,13 +16483,13 @@
         <v>1</v>
       </c>
       <c r="F481" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="G481" t="s">
         <v>10</v>
       </c>
       <c r="H481" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="482">
@@ -16494,7 +16497,7 @@
         <v>91</v>
       </c>
       <c r="B482" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C482" t="b">
         <v>1</v>
@@ -16506,13 +16509,13 @@
         <v>1</v>
       </c>
       <c r="F482" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="G482" t="s">
         <v>10</v>
       </c>
       <c r="H482" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="483">
@@ -16520,7 +16523,7 @@
         <v>105</v>
       </c>
       <c r="B483" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C483" t="b">
         <v>1</v>
@@ -16532,13 +16535,13 @@
         <v>1</v>
       </c>
       <c r="F483" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="G483" t="s">
         <v>10</v>
       </c>
       <c r="H483" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="484">
@@ -16546,7 +16549,7 @@
         <v>189</v>
       </c>
       <c r="B484" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C484" t="b">
         <v>1</v>
@@ -16558,13 +16561,13 @@
         <v>1</v>
       </c>
       <c r="F484" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="G484" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="H484" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="485">
@@ -16572,7 +16575,7 @@
         <v>196</v>
       </c>
       <c r="B485" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C485" t="b">
         <v>1</v>
@@ -16584,13 +16587,13 @@
         <v>1</v>
       </c>
       <c r="F485" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="G485" t="s">
         <v>10</v>
       </c>
       <c r="H485" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="486">
@@ -16598,7 +16601,7 @@
         <v>203</v>
       </c>
       <c r="B486" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C486" t="b">
         <v>1</v>
@@ -16610,13 +16613,13 @@
         <v>1</v>
       </c>
       <c r="F486" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="G486" t="s">
         <v>143</v>
       </c>
       <c r="H486" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="487">
@@ -16624,7 +16627,7 @@
         <v>210</v>
       </c>
       <c r="B487" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C487" t="b">
         <v>1</v>
@@ -16636,7 +16639,7 @@
         <v>1</v>
       </c>
       <c r="F487" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="G487" t="s">
         <v>10</v>
@@ -16650,7 +16653,7 @@
         <v>217</v>
       </c>
       <c r="B488" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C488" t="b">
         <v>1</v>
@@ -16662,13 +16665,13 @@
         <v>1</v>
       </c>
       <c r="F488" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="G488" t="s">
         <v>10</v>
       </c>
       <c r="H488" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="489">
@@ -16676,7 +16679,7 @@
         <v>224</v>
       </c>
       <c r="B489" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C489" t="b">
         <v>1</v>
@@ -16688,13 +16691,13 @@
         <v>1</v>
       </c>
       <c r="F489" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="G489" t="s">
         <v>10</v>
       </c>
       <c r="H489" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="490">
@@ -16702,7 +16705,7 @@
         <v>231</v>
       </c>
       <c r="B490" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C490" t="b">
         <v>1</v>
@@ -16714,13 +16717,13 @@
         <v>2</v>
       </c>
       <c r="F490" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="G490" t="s">
         <v>10</v>
       </c>
       <c r="H490" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="491">
@@ -16728,7 +16731,7 @@
         <v>238</v>
       </c>
       <c r="B491" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C491" t="b">
         <v>1</v>
@@ -16740,7 +16743,7 @@
         <v>1</v>
       </c>
       <c r="F491" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="G491" t="s">
         <v>73</v>
@@ -16754,7 +16757,7 @@
         <v>245</v>
       </c>
       <c r="B492" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C492" t="b">
         <v>1</v>
@@ -16766,13 +16769,13 @@
         <v>2</v>
       </c>
       <c r="F492" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="G492" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="H492" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="493">
@@ -16780,7 +16783,7 @@
         <v>259</v>
       </c>
       <c r="B493" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C493" t="b">
         <v>1</v>
@@ -16792,13 +16795,13 @@
         <v>1</v>
       </c>
       <c r="F493" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="G493" t="s">
         <v>143</v>
       </c>
       <c r="H493" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="494">
@@ -16806,7 +16809,7 @@
         <v>266</v>
       </c>
       <c r="B494" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C494" t="b">
         <v>1</v>
@@ -16824,7 +16827,7 @@
         <v>10</v>
       </c>
       <c r="H494" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="495">
@@ -16832,7 +16835,7 @@
         <v>273</v>
       </c>
       <c r="B495" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C495" t="b">
         <v>1</v>
@@ -16844,13 +16847,13 @@
         <v>1</v>
       </c>
       <c r="F495" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="G495" t="s">
         <v>143</v>
       </c>
       <c r="H495" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="496">
@@ -16858,7 +16861,7 @@
         <v>280</v>
       </c>
       <c r="B496" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C496" t="b">
         <v>1</v>
@@ -16876,7 +16879,7 @@
         <v>10</v>
       </c>
       <c r="H496" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="497">
@@ -16884,7 +16887,7 @@
         <v>287</v>
       </c>
       <c r="B497" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C497" t="b">
         <v>1</v>
@@ -16896,13 +16899,13 @@
         <v>1</v>
       </c>
       <c r="F497" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="G497" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="H497" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="498">
@@ -16910,7 +16913,7 @@
         <v>294</v>
       </c>
       <c r="B498" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C498" t="b">
         <v>1</v>
@@ -16922,13 +16925,13 @@
         <v>1</v>
       </c>
       <c r="F498" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G498" t="s">
         <v>605</v>
       </c>
       <c r="H498" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="499">
@@ -16936,7 +16939,7 @@
         <v>301</v>
       </c>
       <c r="B499" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C499" t="b">
         <v>1</v>
@@ -16948,13 +16951,13 @@
         <v>1</v>
       </c>
       <c r="F499" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="G499" t="s">
         <v>10</v>
       </c>
       <c r="H499" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="500">
@@ -16962,7 +16965,7 @@
         <v>322</v>
       </c>
       <c r="B500" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C500" t="b">
         <v>1</v>
@@ -16974,13 +16977,13 @@
         <v>1</v>
       </c>
       <c r="F500" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="G500" t="s">
         <v>10</v>
       </c>
       <c r="H500" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="501">
@@ -16988,7 +16991,7 @@
         <v>343</v>
       </c>
       <c r="B501" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C501" t="b">
         <v>1</v>
@@ -17000,7 +17003,7 @@
         <v>1</v>
       </c>
       <c r="F501" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="G501" t="s">
         <v>10</v>
@@ -17014,7 +17017,7 @@
         <v>350</v>
       </c>
       <c r="B502" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C502" t="b">
         <v>1</v>
@@ -17026,13 +17029,13 @@
         <v>1</v>
       </c>
       <c r="F502" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="G502" t="s">
         <v>10</v>
       </c>
       <c r="H502" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="503">
@@ -17040,7 +17043,7 @@
         <v>357</v>
       </c>
       <c r="B503" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C503" t="b">
         <v>1</v>
@@ -17058,7 +17061,7 @@
         <v>10</v>
       </c>
       <c r="H503" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="504">
@@ -17066,7 +17069,7 @@
         <v>371</v>
       </c>
       <c r="B504" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C504" t="b">
         <v>1</v>
@@ -17078,13 +17081,13 @@
         <v>1</v>
       </c>
       <c r="F504" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="G504" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="H504" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="505">
@@ -17092,7 +17095,7 @@
         <v>378</v>
       </c>
       <c r="B505" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C505" t="b">
         <v>1</v>
@@ -17110,7 +17113,7 @@
         <v>10</v>
       </c>
       <c r="H505" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="506">
@@ -17118,7 +17121,7 @@
         <v>385</v>
       </c>
       <c r="B506" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C506" t="b">
         <v>1</v>
@@ -17130,13 +17133,13 @@
         <v>1</v>
       </c>
       <c r="F506" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="G506" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="H506" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="507">
@@ -17144,7 +17147,7 @@
         <v>392</v>
       </c>
       <c r="B507" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C507" t="b">
         <v>1</v>
@@ -17156,13 +17159,13 @@
         <v>1</v>
       </c>
       <c r="F507" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="G507" t="s">
         <v>10</v>
       </c>
       <c r="H507" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="508">
@@ -17170,7 +17173,7 @@
         <v>399</v>
       </c>
       <c r="B508" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C508" t="b">
         <v>1</v>
@@ -17188,7 +17191,7 @@
         <v>10</v>
       </c>
       <c r="H508" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="509">
@@ -17196,7 +17199,7 @@
         <v>406</v>
       </c>
       <c r="B509" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C509" t="b">
         <v>1</v>
@@ -17208,13 +17211,13 @@
         <v>1</v>
       </c>
       <c r="F509" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="G509" t="s">
         <v>121</v>
       </c>
       <c r="H509" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="510">
@@ -17222,7 +17225,7 @@
         <v>420</v>
       </c>
       <c r="B510" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C510" t="b">
         <v>1</v>
@@ -17234,13 +17237,13 @@
         <v>1</v>
       </c>
       <c r="F510" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="G510" t="s">
         <v>10</v>
       </c>
       <c r="H510" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="511">
@@ -17248,7 +17251,7 @@
         <v>427</v>
       </c>
       <c r="B511" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C511" t="b">
         <v>1</v>
@@ -17260,13 +17263,13 @@
         <v>1</v>
       </c>
       <c r="F511" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="G511" t="s">
         <v>10</v>
       </c>
       <c r="H511" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="512">
@@ -17274,7 +17277,7 @@
         <v>434</v>
       </c>
       <c r="B512" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C512" t="b">
         <v>1</v>
@@ -17286,13 +17289,13 @@
         <v>1</v>
       </c>
       <c r="F512" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="G512" t="s">
         <v>10</v>
       </c>
       <c r="H512" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="513">
@@ -17300,7 +17303,7 @@
         <v>441</v>
       </c>
       <c r="B513" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C513" t="b">
         <v>1</v>
@@ -17312,13 +17315,13 @@
         <v>1</v>
       </c>
       <c r="F513" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="G513" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="H513" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="514">
@@ -17326,7 +17329,7 @@
         <v>448</v>
       </c>
       <c r="B514" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C514" t="b">
         <v>1</v>
@@ -17338,13 +17341,13 @@
         <v>1</v>
       </c>
       <c r="F514" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="G514" t="s">
         <v>541</v>
       </c>
       <c r="H514" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="515">
@@ -17352,7 +17355,7 @@
         <v>455</v>
       </c>
       <c r="B515" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C515" t="b">
         <v>1</v>
@@ -17364,13 +17367,13 @@
         <v>1</v>
       </c>
       <c r="F515" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="G515" t="s">
         <v>67</v>
       </c>
       <c r="H515" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="516">
@@ -17378,7 +17381,7 @@
         <v>462</v>
       </c>
       <c r="B516" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C516" t="b">
         <v>1</v>
@@ -17390,13 +17393,13 @@
         <v>4</v>
       </c>
       <c r="F516" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="G516" t="s">
         <v>10</v>
       </c>
       <c r="H516" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="517">
@@ -17404,7 +17407,7 @@
         <v>469</v>
       </c>
       <c r="B517" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C517" t="b">
         <v>1</v>
@@ -17422,7 +17425,7 @@
         <v>10</v>
       </c>
       <c r="H517" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="518">
@@ -17430,7 +17433,7 @@
         <v>476</v>
       </c>
       <c r="B518" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C518" t="b">
         <v>1</v>
@@ -17442,13 +17445,13 @@
         <v>1</v>
       </c>
       <c r="F518" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="G518" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="H518" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="519">
@@ -17456,7 +17459,7 @@
         <v>483</v>
       </c>
       <c r="B519" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C519" t="b">
         <v>1</v>
@@ -17468,13 +17471,13 @@
         <v>1</v>
       </c>
       <c r="F519" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="G519" t="s">
         <v>10</v>
       </c>
       <c r="H519" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="520">
@@ -17482,7 +17485,7 @@
         <v>504</v>
       </c>
       <c r="B520" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C520" t="b">
         <v>1</v>
@@ -17494,13 +17497,13 @@
         <v>2</v>
       </c>
       <c r="F520" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="G520" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="H520" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="521">
@@ -17508,7 +17511,7 @@
         <v>513</v>
       </c>
       <c r="B521" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C521" t="b">
         <v>1</v>
@@ -17520,13 +17523,13 @@
         <v>1</v>
       </c>
       <c r="F521" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="G521" t="s">
         <v>10</v>
       </c>
       <c r="H521" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="522">
@@ -17534,7 +17537,7 @@
         <v>520</v>
       </c>
       <c r="B522" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C522" t="b">
         <v>1</v>
@@ -17546,13 +17549,13 @@
         <v>2</v>
       </c>
       <c r="F522" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="G522" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="H522" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="523">
@@ -17560,7 +17563,7 @@
         <v>569</v>
       </c>
       <c r="B523" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C523" t="b">
         <v>1</v>
@@ -17572,13 +17575,13 @@
         <v>1</v>
       </c>
       <c r="F523" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="G523" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="H523" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="524">
@@ -17586,7 +17589,7 @@
         <v>590</v>
       </c>
       <c r="B524" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C524" t="b">
         <v>1</v>
@@ -17598,7 +17601,7 @@
         <v>1</v>
       </c>
       <c r="F524" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="G524" t="s">
         <v>10</v>
@@ -17612,7 +17615,7 @@
         <v>597</v>
       </c>
       <c r="B525" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C525" t="b">
         <v>1</v>
@@ -17624,13 +17627,13 @@
         <v>1</v>
       </c>
       <c r="F525" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="G525" t="s">
         <v>10</v>
       </c>
       <c r="H525" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="526">
@@ -17638,7 +17641,7 @@
         <v>604</v>
       </c>
       <c r="B526" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C526" t="b">
         <v>1</v>
@@ -17650,13 +17653,13 @@
         <v>1</v>
       </c>
       <c r="F526" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="G526" t="s">
         <v>10</v>
       </c>
       <c r="H526" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="527">
@@ -17664,7 +17667,7 @@
         <v>611</v>
       </c>
       <c r="B527" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C527" t="b">
         <v>1</v>
@@ -17676,13 +17679,13 @@
         <v>1</v>
       </c>
       <c r="F527" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="G527" t="s">
         <v>10</v>
       </c>
       <c r="H527" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="528">
@@ -17690,7 +17693,7 @@
         <v>618</v>
       </c>
       <c r="B528" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C528" t="b">
         <v>1</v>
@@ -17702,13 +17705,13 @@
         <v>1</v>
       </c>
       <c r="F528" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="G528" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="H528" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="529">
@@ -17716,7 +17719,7 @@
         <v>632</v>
       </c>
       <c r="B529" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C529" t="b">
         <v>1</v>
@@ -17728,13 +17731,13 @@
         <v>1</v>
       </c>
       <c r="F529" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="G529" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="H529" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="530">
@@ -17742,7 +17745,7 @@
         <v>639</v>
       </c>
       <c r="B530" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C530" t="b">
         <v>1</v>
@@ -17754,13 +17757,13 @@
         <v>1</v>
       </c>
       <c r="F530" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="G530" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="H530" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="531">
@@ -17768,7 +17771,7 @@
         <v>646</v>
       </c>
       <c r="B531" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C531" t="b">
         <v>1</v>
@@ -17786,7 +17789,7 @@
         <v>10</v>
       </c>
       <c r="H531" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="532">
@@ -17794,7 +17797,7 @@
         <v>653</v>
       </c>
       <c r="B532" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C532" t="b">
         <v>1</v>
@@ -17806,13 +17809,13 @@
         <v>1</v>
       </c>
       <c r="F532" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="G532" t="s">
         <v>22</v>
       </c>
       <c r="H532" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="533">
@@ -17820,7 +17823,7 @@
         <v>660</v>
       </c>
       <c r="B533" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C533" t="b">
         <v>1</v>
@@ -17832,13 +17835,13 @@
         <v>1</v>
       </c>
       <c r="F533" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="G533" t="s">
         <v>10</v>
       </c>
       <c r="H533" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="534">
@@ -17846,7 +17849,7 @@
         <v>723</v>
       </c>
       <c r="B534" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C534" t="b">
         <v>1</v>
@@ -17858,13 +17861,13 @@
         <v>1</v>
       </c>
       <c r="F534" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="G534" t="s">
         <v>10</v>
       </c>
       <c r="H534" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="535">
@@ -17872,7 +17875,7 @@
         <v>730</v>
       </c>
       <c r="B535" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C535" t="b">
         <v>1</v>
@@ -17884,13 +17887,13 @@
         <v>1</v>
       </c>
       <c r="F535" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="G535" t="s">
         <v>10</v>
       </c>
       <c r="H535" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="536">
@@ -17898,7 +17901,7 @@
         <v>737</v>
       </c>
       <c r="B536" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C536" t="b">
         <v>1</v>
@@ -17916,7 +17919,7 @@
         <v>10</v>
       </c>
       <c r="H536" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="537">
@@ -17924,7 +17927,7 @@
         <v>744</v>
       </c>
       <c r="B537" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C537" t="b">
         <v>1</v>
@@ -17942,7 +17945,7 @@
         <v>10</v>
       </c>
       <c r="H537" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="538">
@@ -17950,7 +17953,7 @@
         <v>751</v>
       </c>
       <c r="B538" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C538" t="b">
         <v>1</v>
@@ -17962,13 +17965,13 @@
         <v>1</v>
       </c>
       <c r="F538" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="G538" t="s">
         <v>10</v>
       </c>
       <c r="H538" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="539">
@@ -17976,7 +17979,7 @@
         <v>758</v>
       </c>
       <c r="B539" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C539" t="b">
         <v>1</v>
@@ -17988,13 +17991,13 @@
         <v>1</v>
       </c>
       <c r="F539" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="G539" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="H539" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="540">
@@ -18002,7 +18005,7 @@
         <v>765</v>
       </c>
       <c r="B540" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C540" t="b">
         <v>1</v>
@@ -18014,13 +18017,13 @@
         <v>1</v>
       </c>
       <c r="F540" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="G540" t="s">
         <v>10</v>
       </c>
       <c r="H540" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="541">
@@ -18028,7 +18031,7 @@
         <v>772</v>
       </c>
       <c r="B541" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C541" t="b">
         <v>1</v>
@@ -18043,10 +18046,10 @@
         <v>725</v>
       </c>
       <c r="G541" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="H541" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="542">
@@ -18054,7 +18057,7 @@
         <v>779</v>
       </c>
       <c r="B542" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C542" t="b">
         <v>1</v>
@@ -18066,13 +18069,13 @@
         <v>1</v>
       </c>
       <c r="F542" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="G542" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="H542" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="543">
@@ -18080,7 +18083,7 @@
         <v>786</v>
       </c>
       <c r="B543" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C543" t="b">
         <v>1</v>
@@ -18098,7 +18101,7 @@
         <v>10</v>
       </c>
       <c r="H543" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="544">
@@ -18106,7 +18109,7 @@
         <v>800</v>
       </c>
       <c r="B544" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C544" t="b">
         <v>1</v>
@@ -18118,13 +18121,13 @@
         <v>1</v>
       </c>
       <c r="F544" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="G544" t="s">
         <v>10</v>
       </c>
       <c r="H544" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="545">
@@ -18132,7 +18135,7 @@
         <v>807</v>
       </c>
       <c r="B545" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C545" t="b">
         <v>1</v>
@@ -18144,13 +18147,13 @@
         <v>1</v>
       </c>
       <c r="F545" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="G545" t="s">
         <v>10</v>
       </c>
       <c r="H545" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="546">
@@ -18158,7 +18161,7 @@
         <v>814</v>
       </c>
       <c r="B546" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C546" t="b">
         <v>1</v>
@@ -18176,7 +18179,7 @@
         <v>10</v>
       </c>
       <c r="H546" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="547">
@@ -18184,7 +18187,7 @@
         <v>927</v>
       </c>
       <c r="B547" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C547" t="b">
         <v>1</v>
@@ -18196,13 +18199,13 @@
         <v>1</v>
       </c>
       <c r="F547" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="G547" t="s">
         <v>1038</v>
       </c>
       <c r="H547" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="548">
@@ -18210,7 +18213,7 @@
         <v>928</v>
       </c>
       <c r="B548" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C548" t="b">
         <v>1</v>
@@ -18222,13 +18225,13 @@
         <v>1</v>
       </c>
       <c r="F548" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="G548" t="s">
         <v>143</v>
       </c>
       <c r="H548" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="549">
@@ -18236,7 +18239,7 @@
         <v>929</v>
       </c>
       <c r="B549" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C549" t="b">
         <v>1</v>
@@ -18254,7 +18257,7 @@
         <v>10</v>
       </c>
       <c r="H549" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="550">
@@ -18262,7 +18265,7 @@
         <v>932</v>
       </c>
       <c r="B550" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C550" t="b">
         <v>1</v>
@@ -18274,7 +18277,7 @@
         <v>10</v>
       </c>
       <c r="F550" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="G550" t="s">
         <v>121</v>

</xml_diff>